<commit_message>
Added pricing related user stories in the requirements document. Added sheet for monthly forecast in the pricing model(WIP)
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.002.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.002.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="200">
   <si>
     <t>Epics</t>
   </si>
@@ -423,9 +423,6 @@
     <t>As a user I will cancel subscription as to unsubscribe all items from subscription basket.</t>
   </si>
   <si>
-    <t>Generate daily offered price for Subscriptionable item</t>
-  </si>
-  <si>
     <t>As a system I will generate a file on a daily basis containing the itemId, productId, currentOfferedPrice as to provide daily offered price to shopping application.</t>
   </si>
   <si>
@@ -553,9 +550,6 @@
     <t>BEN_06</t>
   </si>
   <si>
-    <t>As a System I will calculate for each product current offered price which is to be offered to anyone subscribing to that product on a given day.</t>
-  </si>
-  <si>
     <t>Item Registration</t>
   </si>
   <si>
@@ -644,6 +638,102 @@
   </si>
   <si>
     <t>Affiance accourdingly update status and other details in the system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create monthly forcast for a product for the duration of one year. </t>
+  </si>
+  <si>
+    <t>Calculate  required metrics for evaluation of product performance</t>
+  </si>
+  <si>
+    <t>PR_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As an administrtor I will forecast following elements related to a product
+1 Purchase price of the product and change in purchase price during the year
+2. Sale price of a product and change in sale price during the year
+3. Number of new customers subscribed for that product every month 
+4. Number of existing customers left subscription every month
+5. Operationl expense incurred for selling the product.
+6. Sales and Marketing expenses incurred for selling the product. </t>
+  </si>
+  <si>
+    <t>As a system I will use the forcasted attributes by administrator and calculate following metrics
+1. Customer churn percentage
+2. Monthly recognized revenue- New
+3..Monthy recognized revenuw - Total
+4. Average revenue per new subscriber
+5. Average revenue per subscriber
+6. Gross margin pecentage
+7. OPerating profit/loass percentage
+8. Subscriber lietime value(SLV)
+9. Cost of acquiring a subscriber(CAS)
+10 SLV/CAS ratio
+11. Period to recover CAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read daily values for the attributes for calculating projections </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a system I will pick up required data based on acuals for calculating projections for a product based on the the dynamics of the product sale.
+Data Picked up 
+1 Purchase price of the product on a day
+2. Sale price of a product on a day
+3. Number of new customers subscribed for that product on a day 
+4. Number of existing customers left subscription on a day
+5. Operationl expense incurred for selling the product on a day.
+6. Sales and Marketing expenses incurred for selling the product on a day. 
+</t>
+  </si>
+  <si>
+    <t>Calculate forecast(projections) based on actual( current and historical) values picked up in earlier user story,using time series analysis.</t>
+  </si>
+  <si>
+    <t>As a system I will use the actual attributes(current and historical)  calculate following metrics for the whole month/year?
+1. Customer churn percentage
+2. Monthly recognized revenue- New
+3..Monthy recognized revenuw - Total
+4. Average revenue per new subscriber
+5. Average revenue per subscriber
+6. Gross margin pecentage
+7. OPerating profit/loass percentage
+8. Subscriber lietime value(SLV)
+9. Cost of acquiring a subscriber(CAS)
+10 SLV/CAS ratio
+11. Period to recover CAS</t>
+  </si>
+  <si>
+    <t>PRI_02</t>
+  </si>
+  <si>
+    <t>PR_03</t>
+  </si>
+  <si>
+    <t>PR_04</t>
+  </si>
+  <si>
+    <t>PR_05</t>
+  </si>
+  <si>
+    <t>PR_06</t>
+  </si>
+  <si>
+    <t>PR_07</t>
+  </si>
+  <si>
+    <t>PR_08</t>
+  </si>
+  <si>
+    <t>PR_09</t>
+  </si>
+  <si>
+    <t>PR_10</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>Compare the projected metrics based on actuals and forecasted metrics and adjust sale price so as to meet the forcast as well as gain required net profit</t>
   </si>
 </sst>
 </file>
@@ -715,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -750,6 +840,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,10 +1602,10 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>19</v>
@@ -1521,13 +1617,13 @@
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>75</v>
@@ -1535,13 +1631,13 @@
     </row>
     <row r="5" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1599,10 +1695,10 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>19</v>
@@ -1614,18 +1710,18 @@
     </row>
     <row r="4" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>70</v>
@@ -1639,7 +1735,7 @@
     </row>
     <row r="6" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>58</v>
@@ -1651,15 +1747,15 @@
         <v>73</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="145" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>68</v>
@@ -1670,27 +1766,27 @@
     </row>
     <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1717,10 +1813,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>19</v>
@@ -1737,7 +1833,7 @@
     </row>
     <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>82</v>
@@ -1745,7 +1841,7 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>83</v>
@@ -1753,7 +1849,7 @@
     </row>
     <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>84</v>
@@ -1761,7 +1857,7 @@
     </row>
     <row r="7" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>22</v>
@@ -1772,7 +1868,7 @@
     </row>
     <row r="8" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
@@ -1783,7 +1879,7 @@
     </row>
     <row r="9" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>26</v>
@@ -1794,7 +1890,7 @@
     </row>
     <row r="10" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>28</v>
@@ -1805,27 +1901,27 @@
     </row>
     <row r="11" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1835,46 +1931,123 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D4"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.7265625" customWidth="1"/>
-    <col min="3" max="3" width="44.26953125" customWidth="1"/>
-    <col min="4" max="4" width="36.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="36.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="68" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>141</v>
+    <row r="4" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>151</v>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1882,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2337,10 +2510,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>19</v>
@@ -2351,7 +2524,7 @@
     </row>
     <row r="2" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>63</v>
@@ -2363,7 +2536,7 @@
     </row>
     <row r="3" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="8" t="s">
@@ -2375,7 +2548,7 @@
     </row>
     <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>65</v>
@@ -2387,7 +2560,7 @@
     </row>
     <row r="5" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="8" t="s">
@@ -2397,7 +2570,7 @@
     </row>
     <row r="6" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>66</v>
@@ -2409,7 +2582,7 @@
     </row>
     <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="8" t="s">
@@ -2442,7 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -2457,25 +2630,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C3" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2486,17 +2659,17 @@
         <v>54</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2504,55 +2677,55 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C11" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C12" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C13" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2560,25 +2733,25 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C20" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C21" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C22" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2604,7 +2777,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2612,7 +2785,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2620,7 +2793,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2628,7 +2801,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2636,7 +2809,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2644,7 +2817,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>